<commit_message>
added project plan, requirements
</commit_message>
<xml_diff>
--- a/docs/WIP/development plan.xlsx
+++ b/docs/WIP/development plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="20730" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="39">
   <si>
     <t>Search</t>
   </si>
@@ -188,12 +188,15 @@
       <t>↓</t>
     </r>
   </si>
+  <si>
+    <t>w11</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,6 +238,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -648,7 +660,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -702,66 +714,75 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1075,7 +1096,7 @@
   <dimension ref="C4:N44"/>
   <sheetViews>
     <sheetView topLeftCell="B28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32:I32"/>
+      <selection activeCell="G32" sqref="D32:I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,37 +1115,37 @@
       <c r="C6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="48">
+      <c r="D6" s="55">
         <v>5</v>
       </c>
-      <c r="E6" s="48">
+      <c r="E6" s="55">
         <v>6</v>
       </c>
-      <c r="F6" s="48">
+      <c r="F6" s="55">
         <v>7</v>
       </c>
-      <c r="G6" s="48">
+      <c r="G6" s="55">
         <v>8</v>
       </c>
-      <c r="H6" s="48">
+      <c r="H6" s="55">
         <v>9</v>
       </c>
-      <c r="I6" s="48">
+      <c r="I6" s="55">
         <v>10</v>
       </c>
-      <c r="J6" s="48">
+      <c r="J6" s="55">
         <v>11</v>
       </c>
-      <c r="K6" s="48">
+      <c r="K6" s="55">
         <v>12</v>
       </c>
-      <c r="L6" s="48">
+      <c r="L6" s="55">
         <v>13</v>
       </c>
-      <c r="M6" s="50">
+      <c r="M6" s="48">
         <v>14</v>
       </c>
-      <c r="N6" s="50" t="s">
+      <c r="N6" s="48" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1132,17 +1153,17 @@
       <c r="C7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="51"/>
-      <c r="N7" s="51"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="56"/>
+      <c r="L7" s="56"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="49"/>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C8" s="5" t="s">
@@ -1380,19 +1401,19 @@
       <c r="M21" s="59"/>
     </row>
     <row r="22" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="54" t="s">
+      <c r="C22" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="55"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="55"/>
-      <c r="I22" s="55"/>
-      <c r="J22" s="55"/>
-      <c r="K22" s="55"/>
-      <c r="L22" s="55"/>
-      <c r="M22" s="56"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="53"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="53"/>
+      <c r="J22" s="53"/>
+      <c r="K22" s="53"/>
+      <c r="L22" s="53"/>
+      <c r="M22" s="54"/>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
@@ -1404,37 +1425,37 @@
       <c r="C27" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="48">
+      <c r="D27" s="55">
         <v>5</v>
       </c>
-      <c r="E27" s="48">
+      <c r="E27" s="55">
         <v>6</v>
       </c>
-      <c r="F27" s="48">
+      <c r="F27" s="55">
         <v>7</v>
       </c>
-      <c r="G27" s="48">
+      <c r="G27" s="55">
         <v>8</v>
       </c>
-      <c r="H27" s="48">
+      <c r="H27" s="55">
         <v>9</v>
       </c>
-      <c r="I27" s="48">
+      <c r="I27" s="55">
         <v>10</v>
       </c>
-      <c r="J27" s="48">
+      <c r="J27" s="55">
         <v>11</v>
       </c>
-      <c r="K27" s="48">
+      <c r="K27" s="55">
         <v>12</v>
       </c>
-      <c r="L27" s="48">
+      <c r="L27" s="55">
         <v>13</v>
       </c>
-      <c r="M27" s="50">
+      <c r="M27" s="48">
         <v>14</v>
       </c>
-      <c r="N27" s="52" t="s">
+      <c r="N27" s="50" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1442,17 +1463,17 @@
       <c r="C28" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="49"/>
-      <c r="I28" s="49"/>
-      <c r="J28" s="49"/>
-      <c r="K28" s="49"/>
-      <c r="L28" s="49"/>
-      <c r="M28" s="51"/>
-      <c r="N28" s="53"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="56"/>
+      <c r="J28" s="56"/>
+      <c r="K28" s="56"/>
+      <c r="L28" s="56"/>
+      <c r="M28" s="49"/>
+      <c r="N28" s="51"/>
     </row>
     <row r="29" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C29" s="5" t="s">
@@ -1514,16 +1535,16 @@
       <c r="C32" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D32" s="45" t="s">
+      <c r="D32" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="E32" s="46"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="45" t="s">
+      <c r="E32" s="61"/>
+      <c r="F32" s="62"/>
+      <c r="G32" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="H32" s="46"/>
-      <c r="I32" s="47"/>
+      <c r="H32" s="61"/>
+      <c r="I32" s="62"/>
       <c r="J32" s="11"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
@@ -1754,6 +1775,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="K27:K28"/>
+    <mergeCell ref="L27:L28"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="G32:I32"/>
     <mergeCell ref="N6:N7"/>
     <mergeCell ref="N27:N28"/>
     <mergeCell ref="C22:M22"/>
@@ -1770,16 +1801,6 @@
     <mergeCell ref="C21:M21"/>
     <mergeCell ref="I27:I28"/>
     <mergeCell ref="J27:J28"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="K27:K28"/>
-    <mergeCell ref="L27:L28"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="G32:I32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -1790,8 +1811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1805,37 +1826,37 @@
       <c r="B4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="48">
+      <c r="C4" s="55">
         <v>5</v>
       </c>
-      <c r="D4" s="48">
+      <c r="D4" s="55">
         <v>6</v>
       </c>
-      <c r="E4" s="48">
+      <c r="E4" s="55">
         <v>7</v>
       </c>
-      <c r="F4" s="48">
+      <c r="F4" s="55">
         <v>8</v>
       </c>
-      <c r="G4" s="48">
+      <c r="G4" s="55">
         <v>9</v>
       </c>
-      <c r="H4" s="48">
+      <c r="H4" s="55">
         <v>10</v>
       </c>
-      <c r="I4" s="48">
+      <c r="I4" s="55">
         <v>11</v>
       </c>
-      <c r="J4" s="48">
+      <c r="J4" s="55">
         <v>12</v>
       </c>
-      <c r="K4" s="48">
+      <c r="K4" s="55">
         <v>13</v>
       </c>
-      <c r="L4" s="50">
+      <c r="L4" s="48">
         <v>14</v>
       </c>
-      <c r="M4" s="52" t="s">
+      <c r="M4" s="50" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1843,17 +1864,17 @@
       <c r="B5" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="53"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="56"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="51"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
@@ -1883,7 +1904,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="33"/>
-      <c r="I7" s="63" t="s">
+      <c r="I7" s="45" t="s">
         <v>17</v>
       </c>
       <c r="J7" s="25"/>
@@ -1915,15 +1936,15 @@
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="60"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="61"/>
-      <c r="K9" s="62"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="64"/>
+      <c r="K9" s="65"/>
       <c r="L9" s="26"/>
       <c r="M9" s="24" t="s">
         <v>26</v>
@@ -2094,7 +2115,7 @@
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="64" t="s">
+      <c r="B19" s="46" t="s">
         <v>30</v>
       </c>
       <c r="C19" s="11"/>
@@ -2112,7 +2133,7 @@
       </c>
     </row>
     <row r="20" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="65" t="s">
+      <c r="B20" s="47" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="21"/>
@@ -2132,7 +2153,7 @@
       </c>
     </row>
     <row r="21" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="65" t="s">
+      <c r="B21" s="47" t="s">
         <v>33</v>
       </c>
       <c r="C21" s="21"/>
@@ -2151,11 +2172,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="M4:M5"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="I9:K9"/>
@@ -2165,6 +2181,11 @@
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M4:M5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2172,12 +2193,391 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B4:N22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N5" sqref="C5:N22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="42.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="55">
+        <v>5</v>
+      </c>
+      <c r="E5" s="55">
+        <v>6</v>
+      </c>
+      <c r="F5" s="55">
+        <v>7</v>
+      </c>
+      <c r="G5" s="55">
+        <v>8</v>
+      </c>
+      <c r="H5" s="55">
+        <v>9</v>
+      </c>
+      <c r="I5" s="55">
+        <v>10</v>
+      </c>
+      <c r="J5" s="55">
+        <v>11</v>
+      </c>
+      <c r="K5" s="55">
+        <v>12</v>
+      </c>
+      <c r="L5" s="55">
+        <v>13</v>
+      </c>
+      <c r="M5" s="48">
+        <v>14</v>
+      </c>
+      <c r="N5" s="50" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="56"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="51"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="25"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="43"/>
+      <c r="N8" s="24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="66"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="61"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="M17" s="28"/>
+      <c r="N17" s="24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C20" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="26"/>
+      <c r="N20" s="31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="J21" s="44"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="35"/>
+      <c r="N21" s="32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>